<commit_message>
Field mapping prototype for 5 templates
</commit_message>
<xml_diff>
--- a/doc_samples/template_4.xlsx
+++ b/doc_samples/template_4.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\IdeaProjects\temp\Excel_documents_data_extraction_and_massaging\doc_samples\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="18060" windowHeight="12660"/>
   </bookViews>
@@ -981,9 +986,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1120,7 +1125,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1306,6 +1311,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1482,20 +1493,24 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1549,6 +1564,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1596,7 +1614,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1631,7 +1649,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1843,19 +1861,19 @@
   <dimension ref="A1:D367"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1868,8 +1886,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
         <v>2000</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1882,8 +1900,8 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>2001</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1896,8 +1914,8 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>2002</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1910,8 +1928,8 @@
         <v>38000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>2003</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1924,8 +1942,8 @@
         <v>9500</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>2004</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1938,8 +1956,8 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>2005</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1952,8 +1970,8 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>2006</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1966,8 +1984,8 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>2007</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1980,8 +1998,8 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>2008</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1994,8 +2012,8 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>2009</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2008,8 +2026,8 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>2010</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2022,8 +2040,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <v>2011</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2036,8 +2054,8 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <v>2012</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2050,8 +2068,8 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
         <v>2013</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -2064,8 +2082,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
         <v>2014</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -2078,8 +2096,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
         <v>2015</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2092,8 +2110,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
         <v>2016</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -2106,8 +2124,8 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
         <v>2017</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2120,8 +2138,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
         <v>2018</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2134,8 +2152,8 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="6">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
         <v>2019</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2148,8 +2166,8 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="6">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
         <v>2020</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2162,8 +2180,8 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="6">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
         <v>2021</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2176,8 +2194,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="6">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
         <v>2022</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -2190,8 +2208,8 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="6">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
         <v>2023</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -2204,8 +2222,8 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="6">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
         <v>2024</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2218,8 +2236,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="6">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
         <v>2025</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2232,8 +2250,8 @@
         <v>13000</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="6">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
         <v>2026</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2246,8 +2264,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="6">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
         <v>2027</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2260,8 +2278,8 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="6">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
         <v>2028</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2274,8 +2292,8 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="6">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
         <v>2029</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2288,8 +2306,8 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="6">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
         <v>2030</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -2302,8 +2320,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="6">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
         <v>2031</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -2316,8 +2334,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="6">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
         <v>2032</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -2330,8 +2348,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="6">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
         <v>2033</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2344,8 +2362,8 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="6">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
         <v>2034</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -2358,8 +2376,8 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="6">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
         <v>2035</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2372,8 +2390,8 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="6">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
         <v>2036</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2386,8 +2404,8 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="6">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
         <v>2037</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -2400,8 +2418,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="6">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
         <v>2038</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -2414,8 +2432,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="6">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
         <v>2039</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -2428,8 +2446,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="6">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
         <v>2040</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -2442,8 +2460,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="6">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
         <v>2041</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -2456,8 +2474,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="6">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
         <v>2042</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -2470,8 +2488,8 @@
         <v>800</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="6">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
         <v>2043</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -2484,8 +2502,8 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="6">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
         <v>2044</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -2498,8 +2516,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="6">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
         <v>2045</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -2512,8 +2530,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="6">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
         <v>2046</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -2526,8 +2544,8 @@
         <v>4800</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="6">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
         <v>2047</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -2540,8 +2558,8 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="6">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
         <v>2048</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -2554,8 +2572,8 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="6">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
         <v>2049</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -2568,8 +2586,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="6">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
         <v>2050</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -2582,8 +2600,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="6">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
         <v>2051</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -2596,8 +2614,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="6">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
         <v>2052</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -2610,8 +2628,8 @@
         <v>300</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="6">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
         <v>2053</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -2624,8 +2642,8 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="6">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
         <v>2054</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -2638,8 +2656,8 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="6">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
         <v>2055</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -2652,8 +2670,8 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="6">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
         <v>2056</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -2666,8 +2684,8 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="6">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
         <v>2057</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -2680,8 +2698,8 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="6">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
         <v>2058</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -2694,8 +2712,8 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="6">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
         <v>2059</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -2708,8 +2726,8 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="6">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
         <v>2060</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -2722,8 +2740,8 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="6">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="7">
         <v>2061</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -2736,8 +2754,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="6">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="7">
         <v>2062</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -2750,8 +2768,8 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="6">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="7">
         <v>2063</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -2764,8 +2782,8 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="6">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="7">
         <v>2064</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -2778,8 +2796,8 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="6">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="7">
         <v>2065</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -2792,8 +2810,8 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="6">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="7">
         <v>2066</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -2806,8 +2824,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="6">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="7">
         <v>2067</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -2820,8 +2838,8 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="6">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="7">
         <v>2068</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -2834,8 +2852,8 @@
         <v>19000</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="6">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="7">
         <v>2069</v>
       </c>
       <c r="B71" s="1" t="s">
@@ -2848,8 +2866,8 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="6">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="7">
         <v>2070</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -2862,8 +2880,8 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="6">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="7">
         <v>2071</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -2876,8 +2894,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="6">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="7">
         <v>2072</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -2890,8 +2908,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="6">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="7">
         <v>2073</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -2904,8 +2922,8 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="6">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="7">
         <v>2074</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -2918,8 +2936,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="6">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="7">
         <v>2075</v>
       </c>
       <c r="B77" s="1" t="s">
@@ -2932,8 +2950,8 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="6">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="7">
         <v>2076</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -2946,8 +2964,8 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="6">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="7">
         <v>2077</v>
       </c>
       <c r="B79" s="1" t="s">
@@ -2960,8 +2978,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="6">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="7">
         <v>2078</v>
       </c>
       <c r="B80" s="1" t="s">
@@ -2974,8 +2992,8 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="6">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="7">
         <v>2079</v>
       </c>
       <c r="B81" s="1" t="s">
@@ -2988,8 +3006,8 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="6">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="7">
         <v>2080</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -3002,8 +3020,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="6">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="7">
         <v>2081</v>
       </c>
       <c r="B83" s="1" t="s">
@@ -3016,8 +3034,8 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="6">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="7">
         <v>2082</v>
       </c>
       <c r="B84" s="1" t="s">
@@ -3030,8 +3048,8 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="6">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="7">
         <v>2083</v>
       </c>
       <c r="B85" s="1" t="s">
@@ -3044,8 +3062,8 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="6">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="7">
         <v>2084</v>
       </c>
       <c r="B86" s="1" t="s">
@@ -3058,8 +3076,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="6">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="7">
         <v>2085</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -3072,8 +3090,8 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" s="6">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="7">
         <v>2086</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -3086,8 +3104,8 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" s="6">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="7">
         <v>2087</v>
       </c>
       <c r="B89" s="1" t="s">
@@ -3100,8 +3118,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" s="6">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="7">
         <v>2088</v>
       </c>
       <c r="B90" s="1" t="s">
@@ -3114,8 +3132,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" s="6">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="7">
         <v>2089</v>
       </c>
       <c r="B91" s="1" t="s">
@@ -3128,8 +3146,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" s="6">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="7">
         <v>2090</v>
       </c>
       <c r="B92" s="1" t="s">
@@ -3142,8 +3160,8 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" s="6">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="7">
         <v>2091</v>
       </c>
       <c r="B93" s="1" t="s">
@@ -3156,8 +3174,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" s="6">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="7">
         <v>2092</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -3170,8 +3188,8 @@
         <v>700</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" s="6">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="7">
         <v>2093</v>
       </c>
       <c r="B95" s="1" t="s">
@@ -3184,8 +3202,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" s="6">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="7">
         <v>2094</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -3198,8 +3216,8 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" s="6">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="7">
         <v>2095</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -3212,8 +3230,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" s="6">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="7">
         <v>2096</v>
       </c>
       <c r="B98" s="1" t="s">
@@ -3226,8 +3244,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" s="6">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="7">
         <v>2097</v>
       </c>
       <c r="B99" s="1" t="s">
@@ -3240,8 +3258,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" s="6">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="7">
         <v>2098</v>
       </c>
       <c r="B100" s="1" t="s">
@@ -3254,8 +3272,8 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" s="6">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="7">
         <v>2099</v>
       </c>
       <c r="B101" s="1" t="s">
@@ -3268,8 +3286,8 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" s="6">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="7">
         <v>2100</v>
       </c>
       <c r="B102" s="1" t="s">
@@ -3282,8 +3300,8 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" s="6">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="7">
         <v>2101</v>
       </c>
       <c r="B103" s="1" t="s">
@@ -3296,8 +3314,8 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" s="6">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="7">
         <v>2102</v>
       </c>
       <c r="B104" s="1" t="s">
@@ -3310,8 +3328,8 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105" s="6">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="7">
         <v>2103</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -3324,8 +3342,8 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106" s="6">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="7">
         <v>2104</v>
       </c>
       <c r="B106" s="1" t="s">
@@ -3338,8 +3356,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A107" s="6">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="7">
         <v>2105</v>
       </c>
       <c r="B107" s="1" t="s">
@@ -3352,8 +3370,8 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108" s="6">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="7">
         <v>2106</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -3366,8 +3384,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A109" s="6">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="7">
         <v>2107</v>
       </c>
       <c r="B109" s="1" t="s">
@@ -3380,8 +3398,8 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A110" s="6">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="7">
         <v>2108</v>
       </c>
       <c r="B110" s="1" t="s">
@@ -3394,8 +3412,8 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A111" s="6">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="7">
         <v>2109</v>
       </c>
       <c r="B111" s="1" t="s">
@@ -3408,8 +3426,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A112" s="6">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="7">
         <v>2110</v>
       </c>
       <c r="B112" s="1" t="s">
@@ -3422,8 +3440,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A113" s="6">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="7">
         <v>2111</v>
       </c>
       <c r="B113" s="1" t="s">
@@ -3436,8 +3454,8 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A114" s="6">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="7">
         <v>2112</v>
       </c>
       <c r="B114" s="1" t="s">
@@ -3450,8 +3468,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A115" s="6">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="7">
         <v>2113</v>
       </c>
       <c r="B115" s="1" t="s">
@@ -3464,8 +3482,8 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A116" s="6">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="7">
         <v>2114</v>
       </c>
       <c r="B116" s="1" t="s">
@@ -3478,8 +3496,8 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A117" s="6">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="7">
         <v>2115</v>
       </c>
       <c r="B117" s="1" t="s">
@@ -3492,8 +3510,8 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A118" s="6">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="7">
         <v>2116</v>
       </c>
       <c r="B118" s="1" t="s">
@@ -3506,8 +3524,8 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A119" s="6">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="7">
         <v>2117</v>
       </c>
       <c r="B119" s="1" t="s">
@@ -3520,8 +3538,8 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A120" s="6">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="7">
         <v>2118</v>
       </c>
       <c r="B120" s="1" t="s">
@@ -3534,8 +3552,8 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A121" s="6">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="7">
         <v>2119</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -3548,8 +3566,8 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A122" s="6">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="7">
         <v>2120</v>
       </c>
       <c r="B122" s="1" t="s">
@@ -3562,8 +3580,8 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A123" s="6">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="7">
         <v>2121</v>
       </c>
       <c r="B123" s="1" t="s">
@@ -3576,8 +3594,8 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A124" s="6">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="7">
         <v>2122</v>
       </c>
       <c r="B124" s="1" t="s">
@@ -3590,8 +3608,8 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A125" s="6">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="7">
         <v>2123</v>
       </c>
       <c r="B125" s="1" t="s">
@@ -3604,8 +3622,8 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A126" s="6">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="7">
         <v>2124</v>
       </c>
       <c r="B126" s="1" t="s">
@@ -3618,8 +3636,8 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A127" s="6">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="7">
         <v>2125</v>
       </c>
       <c r="B127" s="1" t="s">
@@ -3632,8 +3650,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A128" s="6">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="7">
         <v>2126</v>
       </c>
       <c r="B128" s="1" t="s">
@@ -3646,8 +3664,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A129" s="6">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="7">
         <v>2127</v>
       </c>
       <c r="B129" s="1" t="s">
@@ -3660,8 +3678,8 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A130" s="6">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="7">
         <v>2128</v>
       </c>
       <c r="B130" s="1" t="s">
@@ -3674,8 +3692,8 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A131" s="6">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="7">
         <v>2129</v>
       </c>
       <c r="B131" s="1" t="s">
@@ -3688,8 +3706,8 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A132" s="6">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="7">
         <v>2130</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -3702,8 +3720,8 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A133" s="6">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="7">
         <v>2131</v>
       </c>
       <c r="B133" s="1" t="s">
@@ -3716,8 +3734,8 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A134" s="6">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="7">
         <v>2132</v>
       </c>
       <c r="B134" s="1" t="s">
@@ -3730,8 +3748,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A135" s="6">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="7">
         <v>2133</v>
       </c>
       <c r="B135" s="1" t="s">
@@ -3744,8 +3762,8 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A136" s="6">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="7">
         <v>2134</v>
       </c>
       <c r="B136" s="1" t="s">
@@ -3758,8 +3776,8 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A137" s="6">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="7">
         <v>2135</v>
       </c>
       <c r="B137" s="1" t="s">
@@ -3772,8 +3790,8 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A138" s="6">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="7">
         <v>2136</v>
       </c>
       <c r="B138" s="1" t="s">
@@ -3786,8 +3804,8 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A139" s="6">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="7">
         <v>2137</v>
       </c>
       <c r="B139" s="1" t="s">
@@ -3800,8 +3818,8 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A140" s="6">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="7">
         <v>2138</v>
       </c>
       <c r="B140" s="1" t="s">
@@ -3814,8 +3832,8 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A141" s="6">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="7">
         <v>2139</v>
       </c>
       <c r="B141" s="1" t="s">
@@ -3828,8 +3846,8 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A142" s="6">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="7">
         <v>2140</v>
       </c>
       <c r="B142" s="1" t="s">
@@ -3842,8 +3860,8 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A143" s="6">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="7">
         <v>2141</v>
       </c>
       <c r="B143" s="1" t="s">
@@ -3856,8 +3874,8 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A144" s="6">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="7">
         <v>2142</v>
       </c>
       <c r="B144" s="1" t="s">
@@ -3870,8 +3888,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A145" s="6">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="7">
         <v>2143</v>
       </c>
       <c r="B145" s="1" t="s">
@@ -3884,8 +3902,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A146" s="6">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="7">
         <v>2144</v>
       </c>
       <c r="B146" s="1" t="s">
@@ -3898,8 +3916,8 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A147" s="6">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="7">
         <v>2145</v>
       </c>
       <c r="B147" s="1" t="s">
@@ -3912,8 +3930,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A148" s="6">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="7">
         <v>2146</v>
       </c>
       <c r="B148" s="1" t="s">
@@ -3926,8 +3944,8 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A149" s="6">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="7">
         <v>2147</v>
       </c>
       <c r="B149" s="1" t="s">
@@ -3940,8 +3958,8 @@
         <v>900</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A150" s="6">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="7">
         <v>2148</v>
       </c>
       <c r="B150" s="1" t="s">
@@ -3954,8 +3972,8 @@
         <v>900</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A151" s="6">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="7">
         <v>2149</v>
       </c>
       <c r="B151" s="1" t="s">
@@ -3968,8 +3986,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A152" s="6">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="7">
         <v>2150</v>
       </c>
       <c r="B152" s="1" t="s">
@@ -3982,8 +4000,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A153" s="6">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="7">
         <v>2151</v>
       </c>
       <c r="B153" s="1" t="s">
@@ -3996,8 +4014,8 @@
         <v>500</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A154" s="6">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="7">
         <v>2152</v>
       </c>
       <c r="B154" s="1" t="s">
@@ -4010,8 +4028,8 @@
         <v>950</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A155" s="6">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="7">
         <v>2153</v>
       </c>
       <c r="B155" s="1" t="s">
@@ -4024,8 +4042,8 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A156" s="6">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="7">
         <v>2154</v>
       </c>
       <c r="B156" s="1" t="s">
@@ -4038,8 +4056,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A157" s="6">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="7">
         <v>2155</v>
       </c>
       <c r="B157" s="1" t="s">
@@ -4052,8 +4070,8 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A158" s="6">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="7">
         <v>2156</v>
       </c>
       <c r="B158" s="1" t="s">
@@ -4066,8 +4084,8 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A159" s="6">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="7">
         <v>2157</v>
       </c>
       <c r="B159" s="1" t="s">
@@ -4080,8 +4098,8 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A160" s="6">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="7">
         <v>2158</v>
       </c>
       <c r="B160" s="1" t="s">
@@ -4094,8 +4112,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A161" s="6">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="7">
         <v>2159</v>
       </c>
       <c r="B161" s="1" t="s">
@@ -4108,8 +4126,8 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A162" s="6">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="7">
         <v>2160</v>
       </c>
       <c r="B162" s="1" t="s">
@@ -4122,8 +4140,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A163" s="6">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="7">
         <v>2161</v>
       </c>
       <c r="B163" s="1" t="s">
@@ -4136,8 +4154,8 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A164" s="6">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="7">
         <v>2162</v>
       </c>
       <c r="B164" s="1" t="s">
@@ -4150,8 +4168,8 @@
         <v>450</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A165" s="6">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="7">
         <v>2163</v>
       </c>
       <c r="B165" s="1" t="s">
@@ -4164,8 +4182,8 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A166" s="6">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="7">
         <v>2164</v>
       </c>
       <c r="B166" s="1" t="s">
@@ -4178,8 +4196,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A167" s="6">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="7">
         <v>2165</v>
       </c>
       <c r="B167" s="1" t="s">
@@ -4192,8 +4210,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A168" s="6">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="7">
         <v>2166</v>
       </c>
       <c r="B168" s="1" t="s">
@@ -4206,8 +4224,8 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A169" s="6">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="7">
         <v>2167</v>
       </c>
       <c r="B169" s="1" t="s">
@@ -4220,8 +4238,8 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A170" s="6">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="7">
         <v>2168</v>
       </c>
       <c r="B170" s="1" t="s">
@@ -4234,8 +4252,8 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A171" s="6">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="7">
         <v>2169</v>
       </c>
       <c r="B171" s="1" t="s">
@@ -4248,8 +4266,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A172" s="6">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="7">
         <v>2170</v>
       </c>
       <c r="B172" s="1" t="s">
@@ -4262,8 +4280,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A173" s="6">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="7">
         <v>2171</v>
       </c>
       <c r="B173" s="1" t="s">
@@ -4276,8 +4294,8 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A174" s="6">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="7">
         <v>2172</v>
       </c>
       <c r="B174" s="1" t="s">
@@ -4290,8 +4308,8 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A175" s="6">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="7">
         <v>2173</v>
       </c>
       <c r="B175" s="1" t="s">
@@ -4304,8 +4322,8 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A176" s="6">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="7">
         <v>2174</v>
       </c>
       <c r="B176" s="1" t="s">
@@ -4318,8 +4336,8 @@
         <v>700</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A177" s="6">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="7">
         <v>2175</v>
       </c>
       <c r="B177" s="1" t="s">
@@ -4332,8 +4350,8 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A178" s="6">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="7">
         <v>2176</v>
       </c>
       <c r="B178" s="1" t="s">
@@ -4346,8 +4364,8 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A179" s="6">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="7">
         <v>2177</v>
       </c>
       <c r="B179" s="1" t="s">
@@ -4360,8 +4378,8 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A180" s="6">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="7">
         <v>2178</v>
       </c>
       <c r="B180" s="1" t="s">
@@ -4374,8 +4392,8 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A181" s="6">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="7">
         <v>2179</v>
       </c>
       <c r="B181" s="1" t="s">
@@ -4388,8 +4406,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A182" s="6">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="7">
         <v>2180</v>
       </c>
       <c r="B182" s="1" t="s">
@@ -4402,8 +4420,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A183" s="6">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="7">
         <v>2181</v>
       </c>
       <c r="B183" s="1" t="s">
@@ -4416,8 +4434,8 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A184" s="6">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="7">
         <v>2182</v>
       </c>
       <c r="B184" s="1" t="s">
@@ -4430,8 +4448,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A185" s="6">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="7">
         <v>2183</v>
       </c>
       <c r="B185" s="1" t="s">
@@ -4444,8 +4462,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A186" s="6">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="7">
         <v>2184</v>
       </c>
       <c r="B186" s="1" t="s">
@@ -4458,8 +4476,8 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A187" s="6">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="7">
         <v>2185</v>
       </c>
       <c r="B187" s="1" t="s">
@@ -4472,8 +4490,8 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A188" s="6">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="7">
         <v>2186</v>
       </c>
       <c r="B188" s="1" t="s">
@@ -4486,8 +4504,8 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A189" s="6">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="7">
         <v>2187</v>
       </c>
       <c r="B189" s="1" t="s">
@@ -4500,8 +4518,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A190" s="6">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="7">
         <v>2188</v>
       </c>
       <c r="B190" s="1" t="s">
@@ -4514,8 +4532,8 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A191" s="6">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="7">
         <v>2189</v>
       </c>
       <c r="B191" s="1" t="s">
@@ -4528,8 +4546,8 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A192" s="6">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="7">
         <v>2190</v>
       </c>
       <c r="B192" s="1" t="s">
@@ -4542,8 +4560,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A193" s="6">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="7">
         <v>2191</v>
       </c>
       <c r="B193" s="1" t="s">
@@ -4556,8 +4574,8 @@
         <v>350</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A194" s="6">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="7">
         <v>2192</v>
       </c>
       <c r="B194" s="1" t="s">
@@ -4570,8 +4588,8 @@
         <v>400</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A195" s="6">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="7">
         <v>2193</v>
       </c>
       <c r="B195" s="1" t="s">
@@ -4584,8 +4602,8 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A196" s="6">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="7">
         <v>2194</v>
       </c>
       <c r="B196" s="1" t="s">
@@ -4598,8 +4616,8 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A197" s="6">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="7">
         <v>2195</v>
       </c>
       <c r="B197" s="1" t="s">
@@ -4612,8 +4630,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A198" s="6">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="7">
         <v>2196</v>
       </c>
       <c r="B198" s="1" t="s">
@@ -4626,8 +4644,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A199" s="6">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="7">
         <v>2197</v>
       </c>
       <c r="B199" s="1" t="s">
@@ -4640,8 +4658,8 @@
         <v>900</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A200" s="6">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="7">
         <v>2198</v>
       </c>
       <c r="B200" s="1" t="s">
@@ -4654,8 +4672,8 @@
         <v>700</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A201" s="6">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="7">
         <v>2199</v>
       </c>
       <c r="B201" s="1" t="s">
@@ -4668,8 +4686,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A202" s="6">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="7">
         <v>2200</v>
       </c>
       <c r="B202" s="1" t="s">
@@ -4682,8 +4700,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A203" s="6">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="7">
         <v>2201</v>
       </c>
       <c r="B203" s="1" t="s">
@@ -4696,8 +4714,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A204" s="6">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="7">
         <v>2202</v>
       </c>
       <c r="B204" s="1" t="s">
@@ -4710,8 +4728,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A205" s="6">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="7">
         <v>2203</v>
       </c>
       <c r="B205" s="1" t="s">
@@ -4724,8 +4742,8 @@
         <v>300</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A206" s="6">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="7">
         <v>2204</v>
       </c>
       <c r="B206" s="1" t="s">
@@ -4738,8 +4756,8 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A207" s="6">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="7">
         <v>2205</v>
       </c>
       <c r="B207" s="1" t="s">
@@ -4752,8 +4770,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A208" s="6">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="7">
         <v>2206</v>
       </c>
       <c r="B208" s="1" t="s">
@@ -4766,8 +4784,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A209" s="6">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" s="7">
         <v>2207</v>
       </c>
       <c r="B209" s="1" t="s">
@@ -4780,8 +4798,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A210" s="6">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="7">
         <v>2208</v>
       </c>
       <c r="B210" s="1" t="s">
@@ -4794,8 +4812,8 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A211" s="6">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="7">
         <v>2209</v>
       </c>
       <c r="B211" s="1" t="s">
@@ -4808,8 +4826,8 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A212" s="6">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="7">
         <v>2210</v>
       </c>
       <c r="B212" s="1" t="s">
@@ -4822,8 +4840,8 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A213" s="6">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="7">
         <v>2211</v>
       </c>
       <c r="B213" s="1" t="s">
@@ -4836,8 +4854,8 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A214" s="6">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="7">
         <v>2212</v>
       </c>
       <c r="B214" s="1" t="s">
@@ -4850,8 +4868,8 @@
         <v>300</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A215" s="6">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" s="7">
         <v>2213</v>
       </c>
       <c r="B215" s="1" t="s">
@@ -4864,8 +4882,8 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A216" s="6">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" s="7">
         <v>2214</v>
       </c>
       <c r="B216" s="1" t="s">
@@ -4878,8 +4896,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A217" s="6">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" s="7">
         <v>2215</v>
       </c>
       <c r="B217" s="1" t="s">
@@ -4892,8 +4910,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A218" s="6">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" s="7">
         <v>2216</v>
       </c>
       <c r="B218" s="1" t="s">
@@ -4906,8 +4924,8 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A219" s="6">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" s="7">
         <v>2217</v>
       </c>
       <c r="B219" s="1" t="s">
@@ -4920,8 +4938,8 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A220" s="6">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220" s="7">
         <v>2218</v>
       </c>
       <c r="B220" s="1" t="s">
@@ -4934,8 +4952,8 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A221" s="6">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" s="7">
         <v>2219</v>
       </c>
       <c r="B221" s="1" t="s">
@@ -4948,8 +4966,8 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A222" s="6">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" s="7">
         <v>2220</v>
       </c>
       <c r="B222" s="1" t="s">
@@ -4962,8 +4980,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A223" s="6">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" s="7">
         <v>2221</v>
       </c>
       <c r="B223" s="1" t="s">
@@ -4976,8 +4994,8 @@
         <v>550</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A224" s="6">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" s="7">
         <v>2222</v>
       </c>
       <c r="B224" s="1" t="s">
@@ -4990,8 +5008,8 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A225" s="6">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" s="7">
         <v>2223</v>
       </c>
       <c r="B225" s="1" t="s">
@@ -5004,8 +5022,8 @@
         <v>300</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A226" s="6">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" s="7">
         <v>2224</v>
       </c>
       <c r="B226" s="1" t="s">
@@ -5018,8 +5036,8 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A227" s="6">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" s="7">
         <v>2225</v>
       </c>
       <c r="B227" s="1" t="s">
@@ -5032,8 +5050,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A228" s="6">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" s="7">
         <v>2226</v>
       </c>
       <c r="B228" s="1" t="s">
@@ -5046,8 +5064,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A229" s="6">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" s="7">
         <v>2227</v>
       </c>
       <c r="B229" s="1" t="s">
@@ -5060,8 +5078,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A230" s="6">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" s="7">
         <v>2228</v>
       </c>
       <c r="B230" s="1" t="s">
@@ -5074,8 +5092,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A231" s="6">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" s="7">
         <v>2229</v>
       </c>
       <c r="B231" s="1" t="s">
@@ -5088,8 +5106,8 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A232" s="6">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" s="7">
         <v>2230</v>
       </c>
       <c r="B232" s="1" t="s">
@@ -5102,8 +5120,8 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A233" s="6">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" s="7">
         <v>2231</v>
       </c>
       <c r="B233" s="1" t="s">
@@ -5116,8 +5134,8 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A234" s="6">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" s="7">
         <v>2232</v>
       </c>
       <c r="B234" s="1" t="s">
@@ -5130,8 +5148,8 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A235" s="6">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" s="7">
         <v>2233</v>
       </c>
       <c r="B235" s="1" t="s">
@@ -5144,8 +5162,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A236" s="6">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" s="7">
         <v>2234</v>
       </c>
       <c r="B236" s="1" t="s">
@@ -5158,8 +5176,8 @@
         <v>550</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A237" s="6">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" s="7">
         <v>2235</v>
       </c>
       <c r="B237" s="1" t="s">
@@ -5172,8 +5190,8 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A238" s="6">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238" s="7">
         <v>2236</v>
       </c>
       <c r="B238" s="1" t="s">
@@ -5186,8 +5204,8 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A239" s="6">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239" s="7">
         <v>2237</v>
       </c>
       <c r="B239" s="1" t="s">
@@ -5200,8 +5218,8 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A240" s="6">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" s="7">
         <v>2238</v>
       </c>
       <c r="B240" s="1" t="s">
@@ -5214,8 +5232,8 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A241" s="6">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" s="7">
         <v>2239</v>
       </c>
       <c r="B241" s="1" t="s">
@@ -5228,8 +5246,8 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A242" s="6">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="7">
         <v>2240</v>
       </c>
       <c r="B242" s="1" t="s">
@@ -5242,8 +5260,8 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A243" s="6">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" s="7">
         <v>2241</v>
       </c>
       <c r="B243" s="1" t="s">
@@ -5256,8 +5274,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A244" s="6">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" s="7">
         <v>2242</v>
       </c>
       <c r="B244" s="1" t="s">
@@ -5270,8 +5288,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A245" s="6">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" s="7">
         <v>2243</v>
       </c>
       <c r="B245" s="1" t="s">
@@ -5284,8 +5302,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A246" s="6">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246" s="7">
         <v>2244</v>
       </c>
       <c r="B246" s="1" t="s">
@@ -5298,8 +5316,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A247" s="6">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" s="7">
         <v>2245</v>
       </c>
       <c r="B247" s="1" t="s">
@@ -5312,8 +5330,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A248" s="6">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" s="7">
         <v>2246</v>
       </c>
       <c r="B248" s="1" t="s">
@@ -5326,8 +5344,8 @@
         <v>400</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A249" s="6">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" s="7">
         <v>2247</v>
       </c>
       <c r="B249" s="1" t="s">
@@ -5340,8 +5358,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A250" s="6">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" s="7">
         <v>2248</v>
       </c>
       <c r="B250" s="1" t="s">
@@ -5354,8 +5372,8 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A251" s="6">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251" s="7">
         <v>2249</v>
       </c>
       <c r="B251" s="1" t="s">
@@ -5368,8 +5386,8 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A252" s="6">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" s="7">
         <v>2250</v>
       </c>
       <c r="B252" s="1" t="s">
@@ -5382,8 +5400,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A253" s="6">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" s="7">
         <v>2251</v>
       </c>
       <c r="B253" s="1" t="s">
@@ -5396,8 +5414,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A254" s="6">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254" s="7">
         <v>2252</v>
       </c>
       <c r="B254" s="1" t="s">
@@ -5410,8 +5428,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A255" s="6">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" s="7">
         <v>2253</v>
       </c>
       <c r="B255" s="1" t="s">
@@ -5424,8 +5442,8 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A256" s="6">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" s="7">
         <v>2254</v>
       </c>
       <c r="B256" s="1" t="s">
@@ -5438,8 +5456,8 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A257" s="6">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" s="7">
         <v>2255</v>
       </c>
       <c r="B257" s="1" t="s">
@@ -5452,8 +5470,8 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A258" s="6">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" s="7">
         <v>2256</v>
       </c>
       <c r="B258" s="1" t="s">
@@ -5466,8 +5484,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A259" s="6">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" s="7">
         <v>2257</v>
       </c>
       <c r="B259" s="1" t="s">
@@ -5480,8 +5498,8 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A260" s="6">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" s="7">
         <v>2258</v>
       </c>
       <c r="B260" s="1" t="s">
@@ -5494,8 +5512,8 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A261" s="6">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" s="7">
         <v>2259</v>
       </c>
       <c r="B261" s="1" t="s">
@@ -5508,8 +5526,8 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A262" s="6">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" s="7">
         <v>2260</v>
       </c>
       <c r="B262" s="1" t="s">
@@ -5522,8 +5540,8 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A263" s="6">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" s="7">
         <v>2261</v>
       </c>
       <c r="B263" s="1" t="s">
@@ -5536,8 +5554,8 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A264" s="6">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264" s="7">
         <v>2262</v>
       </c>
       <c r="B264" s="1" t="s">
@@ -5550,8 +5568,8 @@
         <v>4250</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A265" s="6">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" s="7">
         <v>2263</v>
       </c>
       <c r="B265" s="1" t="s">
@@ -5564,8 +5582,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A266" s="6">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" s="7">
         <v>2264</v>
       </c>
       <c r="B266" s="1" t="s">
@@ -5578,8 +5596,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A267" s="6">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A267" s="7">
         <v>2265</v>
       </c>
       <c r="B267" s="1" t="s">
@@ -5592,8 +5610,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A268" s="6">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268" s="7">
         <v>2266</v>
       </c>
       <c r="B268" s="1" t="s">
@@ -5606,8 +5624,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A269" s="6">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269" s="7">
         <v>2267</v>
       </c>
       <c r="B269" s="1" t="s">
@@ -5620,8 +5638,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A270" s="6">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" s="7">
         <v>2268</v>
       </c>
       <c r="B270" s="1" t="s">
@@ -5634,8 +5652,8 @@
         <v>900</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A271" s="6">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" s="7">
         <v>2269</v>
       </c>
       <c r="B271" s="1" t="s">
@@ -5648,8 +5666,8 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A272" s="6">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" s="7">
         <v>2270</v>
       </c>
       <c r="B272" s="1" t="s">
@@ -5662,8 +5680,8 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A273" s="6">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" s="7">
         <v>2271</v>
       </c>
       <c r="B273" s="1" t="s">
@@ -5676,8 +5694,8 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A274" s="6">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" s="7">
         <v>2272</v>
       </c>
       <c r="B274" s="1" t="s">
@@ -5690,8 +5708,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A275" s="6">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" s="7">
         <v>2273</v>
       </c>
       <c r="B275" s="1" t="s">
@@ -5704,8 +5722,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A276" s="6">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276" s="7">
         <v>2274</v>
       </c>
       <c r="B276" s="1" t="s">
@@ -5718,8 +5736,8 @@
         <v>9500</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A277" s="6">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A277" s="7">
         <v>2275</v>
       </c>
       <c r="B277" s="1" t="s">
@@ -5732,8 +5750,8 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A278" s="6">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" s="7">
         <v>2276</v>
       </c>
       <c r="B278" s="1" t="s">
@@ -5746,8 +5764,8 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A279" s="6">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" s="7">
         <v>2277</v>
       </c>
       <c r="B279" s="1" t="s">
@@ -5760,8 +5778,8 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A280" s="6">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A280" s="7">
         <v>2278</v>
       </c>
       <c r="B280" s="1" t="s">
@@ -5774,8 +5792,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A281" s="6">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A281" s="7">
         <v>2279</v>
       </c>
       <c r="B281" s="1" t="s">
@@ -5788,8 +5806,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A282" s="6">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A282" s="7">
         <v>2280</v>
       </c>
       <c r="B282" s="1" t="s">
@@ -5802,8 +5820,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A283" s="6">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" s="7">
         <v>2281</v>
       </c>
       <c r="B283" s="1" t="s">
@@ -5816,8 +5834,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A284" s="6">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A284" s="7">
         <v>2282</v>
       </c>
       <c r="B284" s="1" t="s">
@@ -5830,8 +5848,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A285" s="6">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A285" s="7">
         <v>2283</v>
       </c>
       <c r="B285" s="1" t="s">
@@ -5844,8 +5862,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A286" s="6">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A286" s="7">
         <v>2284</v>
       </c>
       <c r="B286" s="1" t="s">
@@ -5858,8 +5876,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A287" s="6">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A287" s="7">
         <v>2285</v>
       </c>
       <c r="B287" s="1" t="s">
@@ -5872,8 +5890,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A288" s="6">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A288" s="7">
         <v>2286</v>
       </c>
       <c r="B288" s="1" t="s">
@@ -5886,8 +5904,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A289" s="6">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A289" s="7">
         <v>2287</v>
       </c>
       <c r="B289" s="1" t="s">
@@ -5900,8 +5918,8 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A290" s="6">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" s="7">
         <v>2288</v>
       </c>
       <c r="B290" s="1" t="s">
@@ -5914,8 +5932,8 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A291" s="6">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291" s="7">
         <v>2289</v>
       </c>
       <c r="B291" s="1" t="s">
@@ -5928,8 +5946,8 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A292" s="6">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292" s="7">
         <v>2290</v>
       </c>
       <c r="B292" s="1" t="s">
@@ -5942,8 +5960,8 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A293" s="6">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A293" s="7">
         <v>2291</v>
       </c>
       <c r="B293" s="1" t="s">
@@ -5956,8 +5974,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A294" s="6">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A294" s="7">
         <v>2292</v>
       </c>
       <c r="B294" s="1" t="s">
@@ -5970,8 +5988,8 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A295" s="6">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A295" s="7">
         <v>2293</v>
       </c>
       <c r="B295" s="1" t="s">
@@ -5984,8 +6002,8 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A296" s="6">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A296" s="7">
         <v>2294</v>
       </c>
       <c r="B296" s="1" t="s">
@@ -5998,8 +6016,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A297" s="6">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A297" s="7">
         <v>2295</v>
       </c>
       <c r="B297" s="1" t="s">
@@ -6012,8 +6030,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A298" s="6">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A298" s="7">
         <v>2296</v>
       </c>
       <c r="B298" s="1" t="s">
@@ -6026,8 +6044,8 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A299" s="6">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A299" s="7">
         <v>2297</v>
       </c>
       <c r="B299" s="1" t="s">
@@ -6040,8 +6058,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A300" s="6">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A300" s="7">
         <v>2298</v>
       </c>
       <c r="B300" s="1" t="s">
@@ -6054,8 +6072,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A301" s="6">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A301" s="7">
         <v>2299</v>
       </c>
       <c r="B301" s="1" t="s">
@@ -6068,8 +6086,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A302" s="6">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A302" s="7">
         <v>2300</v>
       </c>
       <c r="B302" s="1" t="s">
@@ -6082,8 +6100,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A303" s="6">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A303" s="7">
         <v>2301</v>
       </c>
       <c r="B303" s="1" t="s">
@@ -6096,8 +6114,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A304" s="6">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A304" s="7">
         <v>2302</v>
       </c>
       <c r="B304" s="1" t="s">
@@ -6110,8 +6128,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A305" s="6">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A305" s="7">
         <v>2303</v>
       </c>
       <c r="B305" s="1" t="s">
@@ -6124,8 +6142,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A306" s="6">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A306" s="7">
         <v>2304</v>
       </c>
       <c r="B306" s="1" t="s">
@@ -6138,8 +6156,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A307" s="6">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A307" s="7">
         <v>2305</v>
       </c>
       <c r="B307" s="1" t="s">
@@ -6152,8 +6170,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A308" s="6">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A308" s="7">
         <v>2306</v>
       </c>
       <c r="B308" s="1" t="s">
@@ -6166,8 +6184,8 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A309" s="6">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A309" s="7">
         <v>2307</v>
       </c>
       <c r="B309" s="1" t="s">
@@ -6180,8 +6198,8 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A310" s="6">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A310" s="7">
         <v>2308</v>
       </c>
       <c r="B310" s="1" t="s">
@@ -6194,8 +6212,8 @@
         <v>450</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A311" s="6">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A311" s="7">
         <v>2309</v>
       </c>
       <c r="B311" s="1" t="s">
@@ -6208,8 +6226,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A312" s="6">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A312" s="7">
         <v>2310</v>
       </c>
       <c r="B312" s="1" t="s">
@@ -6222,8 +6240,8 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A313" s="6">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A313" s="7">
         <v>2311</v>
       </c>
       <c r="B313" s="1" t="s">
@@ -6236,8 +6254,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A314" s="6">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A314" s="7">
         <v>2312</v>
       </c>
       <c r="B314" s="1" t="s">
@@ -6250,8 +6268,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A315" s="6">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A315" s="7">
         <v>2313</v>
       </c>
       <c r="B315" s="1" t="s">
@@ -6264,8 +6282,8 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A316" s="6">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A316" s="7">
         <v>2314</v>
       </c>
       <c r="B316" s="1" t="s">
@@ -6278,8 +6296,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A317" s="6">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A317" s="7">
         <v>2315</v>
       </c>
       <c r="B317" s="1" t="s">
@@ -6292,8 +6310,8 @@
         <v>9500</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A318" s="6">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A318" s="7">
         <v>2316</v>
       </c>
       <c r="B318" s="1" t="s">
@@ -6306,8 +6324,8 @@
         <v>700</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A319" s="6">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A319" s="7">
         <v>2317</v>
       </c>
       <c r="B319" s="1" t="s">
@@ -6320,8 +6338,8 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A320" s="6">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A320" s="7">
         <v>2318</v>
       </c>
       <c r="B320" s="1" t="s">
@@ -6334,8 +6352,8 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A321" s="6">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A321" s="7">
         <v>2319</v>
       </c>
       <c r="B321" s="1" t="s">
@@ -6348,8 +6366,8 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A322" s="6">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A322" s="7">
         <v>2320</v>
       </c>
       <c r="B322" s="1" t="s">
@@ -6362,8 +6380,8 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A323" s="6">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A323" s="7">
         <v>2321</v>
       </c>
       <c r="B323" s="1" t="s">
@@ -6376,8 +6394,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A324" s="6">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A324" s="7">
         <v>2322</v>
       </c>
       <c r="B324" s="1" t="s">
@@ -6390,8 +6408,8 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A325" s="6">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A325" s="7">
         <v>2323</v>
       </c>
       <c r="B325" s="1" t="s">
@@ -6404,8 +6422,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A326" s="6">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A326" s="7">
         <v>2324</v>
       </c>
       <c r="B326" s="1" t="s">
@@ -6418,8 +6436,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A327" s="6">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A327" s="7">
         <v>2325</v>
       </c>
       <c r="B327" s="1" t="s">
@@ -6432,8 +6450,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A328" s="6">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A328" s="7">
         <v>2326</v>
       </c>
       <c r="B328" s="1" t="s">
@@ -6446,8 +6464,8 @@
         <v>700</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A329" s="6">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A329" s="7">
         <v>2327</v>
       </c>
       <c r="B329" s="1" t="s">
@@ -6460,8 +6478,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A330" s="6">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A330" s="7">
         <v>2328</v>
       </c>
       <c r="B330" s="1" t="s">
@@ -6474,8 +6492,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A331" s="6">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A331" s="7">
         <v>2329</v>
       </c>
       <c r="B331" s="1" t="s">
@@ -6488,8 +6506,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A332" s="6">
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A332" s="7">
         <v>2330</v>
       </c>
       <c r="B332" s="1" t="s">
@@ -6502,8 +6520,8 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A333" s="6">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A333" s="7">
         <v>2331</v>
       </c>
       <c r="B333" s="1" t="s">
@@ -6516,8 +6534,8 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A334" s="6">
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A334" s="7">
         <v>2332</v>
       </c>
       <c r="B334" s="1" t="s">
@@ -6530,8 +6548,8 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A335" s="6">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A335" s="7">
         <v>2333</v>
       </c>
       <c r="B335" s="1" t="s">
@@ -6544,8 +6562,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A336" s="6">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A336" s="7">
         <v>2334</v>
       </c>
       <c r="B336" s="1" t="s">
@@ -6558,8 +6576,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A337" s="6">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A337" s="7">
         <v>2335</v>
       </c>
       <c r="B337" s="1" t="s">
@@ -6572,8 +6590,8 @@
         <v>800</v>
       </c>
     </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A338" s="6">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A338" s="7">
         <v>2336</v>
       </c>
       <c r="B338" s="1" t="s">
@@ -6586,8 +6604,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A339" s="6">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A339" s="7">
         <v>2337</v>
       </c>
       <c r="B339" s="1" t="s">
@@ -6600,8 +6618,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A340" s="6">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A340" s="7">
         <v>2338</v>
       </c>
       <c r="B340" s="1" t="s">
@@ -6614,8 +6632,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A341" s="6">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A341" s="7">
         <v>2339</v>
       </c>
       <c r="B341" s="1" t="s">
@@ -6628,8 +6646,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A342" s="6">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A342" s="7">
         <v>2340</v>
       </c>
       <c r="B342" s="1" t="s">
@@ -6642,8 +6660,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A343" s="6">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A343" s="7">
         <v>2341</v>
       </c>
       <c r="B343" s="1" t="s">
@@ -6656,8 +6674,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A344" s="6">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A344" s="7">
         <v>2342</v>
       </c>
       <c r="B344" s="1" t="s">
@@ -6670,8 +6688,8 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A345" s="6">
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A345" s="7">
         <v>2343</v>
       </c>
       <c r="B345" s="1" t="s">
@@ -6684,8 +6702,8 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A346" s="6">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A346" s="7">
         <v>2344</v>
       </c>
       <c r="B346" s="1" t="s">
@@ -6698,8 +6716,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A347" s="6">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A347" s="7">
         <v>2345</v>
       </c>
       <c r="B347" s="1" t="s">
@@ -6712,8 +6730,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A348" s="6">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A348" s="7">
         <v>2346</v>
       </c>
       <c r="B348" s="1" t="s">
@@ -6726,8 +6744,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A349" s="6">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A349" s="7">
         <v>2347</v>
       </c>
       <c r="B349" s="1" t="s">
@@ -6740,8 +6758,8 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="350" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A350" s="6">
+    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A350" s="7">
         <v>2348</v>
       </c>
       <c r="B350" s="1" t="s">
@@ -6754,8 +6772,8 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="351" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A351" s="6">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A351" s="7">
         <v>2349</v>
       </c>
       <c r="B351" s="1" t="s">
@@ -6768,8 +6786,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="352" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A352" s="6">
+    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A352" s="7">
         <v>2350</v>
       </c>
       <c r="B352" s="1" t="s">
@@ -6782,8 +6800,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="353" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A353" s="6">
+    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A353" s="7">
         <v>2351</v>
       </c>
       <c r="B353" s="1" t="s">
@@ -6796,8 +6814,8 @@
         <v>500</v>
       </c>
     </row>
-    <row r="354" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A354" s="6">
+    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A354" s="7">
         <v>2352</v>
       </c>
       <c r="B354" s="1" t="s">
@@ -6810,8 +6828,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="355" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A355" s="6">
+    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A355" s="7">
         <v>2353</v>
       </c>
       <c r="B355" s="1" t="s">
@@ -6824,8 +6842,8 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="356" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A356" s="6">
+    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A356" s="7">
         <v>2354</v>
       </c>
       <c r="B356" s="1" t="s">
@@ -6838,8 +6856,8 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="357" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A357" s="6">
+    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A357" s="7">
         <v>2355</v>
       </c>
       <c r="B357" s="1" t="s">
@@ -6852,8 +6870,8 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="358" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A358" s="6">
+    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A358" s="7">
         <v>2356</v>
       </c>
       <c r="B358" s="1" t="s">
@@ -6866,8 +6884,8 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="359" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A359" s="6">
+    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A359" s="7">
         <v>2357</v>
       </c>
       <c r="B359" s="1" t="s">
@@ -6880,8 +6898,8 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="360" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A360" s="6">
+    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A360" s="7">
         <v>2358</v>
       </c>
       <c r="B360" s="1" t="s">
@@ -6894,8 +6912,8 @@
         <v>8500</v>
       </c>
     </row>
-    <row r="361" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A361" s="6">
+    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A361" s="7">
         <v>2359</v>
       </c>
       <c r="B361" s="1" t="s">
@@ -6908,8 +6926,8 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="362" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A362" s="6">
+    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A362" s="7">
         <v>2360</v>
       </c>
       <c r="B362" s="1" t="s">
@@ -6922,8 +6940,8 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="363" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A363" s="6">
+    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A363" s="7">
         <v>2361</v>
       </c>
       <c r="B363" s="1" t="s">
@@ -6936,8 +6954,8 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="364" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A364" s="6">
+    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A364" s="7">
         <v>2362</v>
       </c>
       <c r="B364" s="1" t="s">
@@ -6950,8 +6968,8 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="365" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A365" s="6">
+    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A365" s="7">
         <v>2363</v>
       </c>
       <c r="B365" s="1" t="s">
@@ -6964,8 +6982,8 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A366" s="6">
+    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A366" s="7">
         <v>2364</v>
       </c>
       <c r="B366" s="1" t="s">
@@ -6978,8 +6996,8 @@
         <v>9500</v>
       </c>
     </row>
-    <row r="367" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A367" s="6">
+    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A367" s="7">
         <v>2365</v>
       </c>
       <c r="B367" s="1" t="s">
@@ -7009,7 +7027,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -7021,7 +7039,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>